<commit_message>
update final. global stable v1.2
</commit_message>
<xml_diff>
--- a/excel/import_data.xlsx
+++ b/excel/import_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data training joko\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230A36D2-AC9D-4759-8A8A-CAE589362A79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BFB7F70-7CED-4122-B76C-B2ED95EE3D46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{91CC0114-5978-4487-A5FD-036FA04B730F}"/>
   </bookViews>
@@ -512,7 +512,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,7 +567,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
-        <v>66666</v>
+        <v>11111</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>21</v>
@@ -600,7 +600,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
-        <v>77777</v>
+        <v>22222</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>22</v>
@@ -633,7 +633,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <v>88888</v>
+        <v>33333</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>23</v>
@@ -666,7 +666,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
-        <v>99999</v>
+        <v>44444</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>24</v>
@@ -699,7 +699,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <v>10000</v>
+        <v>55555</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>25</v>

</xml_diff>